<commit_message>
vault backup: 2024-11-16 23:04:27
</commit_message>
<xml_diff>
--- a/学习笔记/深度学习/ViT学习/模型对比1.xlsx
+++ b/学习笔记/深度学习/ViT学习/模型对比1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFiles\obsidian笔记\鸢尾花书学习笔记\学习笔记\深度学习\ViT学习\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA82C89D-590C-4C23-A90C-10D4DA03F9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFF5F57-4218-4E7F-95DF-D46F9441B234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC82C94D-6C04-4121-9F4B-B6E5B714E292}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>